<commit_message>
Update after whole day integration test
</commit_message>
<xml_diff>
--- a/Arduino/Arduino Sensor Raw Data.xlsx
+++ b/Arduino/Arduino Sensor Raw Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="28720" windowHeight="17160" tabRatio="500"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="28720" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>FL</t>
   </si>
@@ -39,9 +39,6 @@
   </si>
   <si>
     <t>fucked</t>
-  </si>
-  <si>
-    <t>200 (fucked alr)</t>
   </si>
   <si>
     <t>SL Target</t>
@@ -85,12 +82,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -109,8 +112,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -395,7 +399,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="C7" sqref="C7:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -414,10 +418,10 @@
         <v>2</v>
       </c>
       <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
         <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -425,16 +429,16 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>625</v>
+        <v>645</v>
       </c>
       <c r="C2">
-        <v>655</v>
+        <v>665</v>
       </c>
       <c r="D2">
-        <v>620</v>
+        <v>642</v>
       </c>
       <c r="G2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H2">
         <v>600</v>
@@ -445,13 +449,13 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B3">
-        <v>400</v>
+        <v>415</v>
       </c>
       <c r="C3">
-        <v>415</v>
+        <v>425</v>
       </c>
       <c r="D3">
-        <v>390</v>
+        <v>410</v>
       </c>
       <c r="G3">
         <v>1.5</v>
@@ -468,13 +472,13 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>295</v>
+        <v>305</v>
       </c>
       <c r="C4">
-        <v>305</v>
+        <v>330</v>
       </c>
       <c r="D4">
-        <v>292</v>
+        <v>300</v>
       </c>
       <c r="G4">
         <v>2</v>
@@ -488,13 +492,13 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B5">
+        <v>245</v>
+      </c>
+      <c r="C5">
+        <v>260</v>
+      </c>
+      <c r="D5">
         <v>235</v>
-      </c>
-      <c r="C5">
-        <v>235</v>
-      </c>
-      <c r="D5">
-        <v>228</v>
       </c>
       <c r="G5">
         <v>2.5</v>
@@ -511,13 +515,13 @@
         <v>3</v>
       </c>
       <c r="B6">
-        <v>190</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
+        <v>200</v>
+      </c>
+      <c r="C6">
+        <v>180</v>
       </c>
       <c r="D6">
-        <v>185</v>
+        <v>199</v>
       </c>
       <c r="G6">
         <v>3</v>
@@ -531,13 +535,13 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B7">
+        <v>165</v>
+      </c>
+      <c r="C7" s="1">
         <v>160</v>
       </c>
-      <c r="C7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7">
-        <v>168</v>
+      <c r="D7" s="1">
+        <v>175</v>
       </c>
       <c r="G7">
         <v>3.5</v>
@@ -554,10 +558,13 @@
         <v>4</v>
       </c>
       <c r="B8">
-        <v>140</v>
-      </c>
-      <c r="D8">
-        <v>155</v>
+        <v>135</v>
+      </c>
+      <c r="C8" s="1">
+        <v>130</v>
+      </c>
+      <c r="D8" s="1">
+        <v>175</v>
       </c>
       <c r="G8">
         <v>4</v>
@@ -571,10 +578,13 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B9">
-        <v>120</v>
-      </c>
-      <c r="D9">
-        <v>140</v>
+        <v>110</v>
+      </c>
+      <c r="C9" s="1">
+        <v>110</v>
+      </c>
+      <c r="D9" s="1">
+        <v>180</v>
       </c>
       <c r="G9">
         <v>4.5</v>
@@ -621,7 +631,7 @@
         <v>6.5</v>
       </c>
       <c r="I13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>